<commit_message>
Updated RegistrationPage class to cast zipcode as integer
</commit_message>
<xml_diff>
--- a/AutomationPractice/src/main/resources/excel/logindata.xlsx
+++ b/AutomationPractice/src/main/resources/excel/logindata.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t xml:space="preserve">batman</t>
+    <t xml:space="preserve">username</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">admin</t>
   </si>
   <si>
-    <t xml:space="preserve">wsad</t>
+    <t xml:space="preserve">adadsd</t>
   </si>
   <si>
     <t xml:space="preserve">jnqwwjndewjd@test.com</t>
@@ -53,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -74,6 +74,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,12 +132,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,10 +175,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -180,7 +191,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -188,7 +199,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -196,7 +207,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">

</xml_diff>